<commit_message>
Added tests with CBMC
</commit_message>
<xml_diff>
--- a/test2/results_13Jul2015/UnitTestingResults.xlsx
+++ b/test2/results_13Jul2015/UnitTestingResults.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -112,7 +113,7 @@
     <t>Analyze how parsing is being executed and check if changing those functions may transform the resulting output out of it.</t>
   </si>
   <si>
-    <t>gopan.c  </t>
+    <t>gopan.c</t>
   </si>
   <si>
     <t>Original unit test file</t>
@@ -145,7 +146,7 @@
     <t>Failed on parsing file anno_terminator_02_true-unreach-call_true-termination.c with same error as test 4.</t>
   </si>
   <si>
-    <t>insertion_sort_true-unreach-call.c </t>
+    <t>insertion_sort_true-unreach-call.c</t>
   </si>
   <si>
     <t>Missed the correct location of while by 2 :(</t>
@@ -160,7 +161,7 @@
     <t>Faled on parsing file anno_terminator_03_false-unreach-call_true-termination.c</t>
   </si>
   <si>
-    <t>linear_sea.ch_true-unreach-call.c  </t>
+    <t>linear_sea.ch_true-unreach-call.c</t>
   </si>
   <si>
     <t>Missed the location of while by 1.</t>
@@ -172,7 +173,7 @@
     <t>Failed on parsing file anno_terminator_03_true-unreach-call_true-termination.c with same error as test 4.</t>
   </si>
   <si>
-    <t>linear_search_false-unreach-call.c </t>
+    <t>linear_search_false-unreach-call.c</t>
   </si>
   <si>
     <t>Invariant comment was misplaced by 1 (line 15 instead of 14 as logged). Also, it was placed before the while and after another comment.</t>
@@ -229,6 +230,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -334,7 +336,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.3367346938776"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5357142857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>